<commit_message>
log normal selling prices and exponential demand added
</commit_message>
<xml_diff>
--- a/unittests/test_sheets/test.xlsx
+++ b/unittests/test_sheets/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>r</t>
   </si>
@@ -39,24 +39,12 @@
     <t>working_capital</t>
   </si>
   <si>
-    <t>selling_price</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
-    <t>mu_consumer_demand</t>
-  </si>
-  <si>
-    <t>sigma_consumer_demand</t>
-  </si>
-  <si>
     <t>p_delivery</t>
   </si>
   <si>
-    <t>max_suppliers</t>
-  </si>
-  <si>
     <t>input_margin</t>
   </si>
   <si>
@@ -67,6 +55,15 @@
   </si>
   <si>
     <t>5.3</t>
+  </si>
+  <si>
+    <t>consumer_demand_mean</t>
+  </si>
+  <si>
+    <t>mu_selling_price</t>
+  </si>
+  <si>
+    <t>sigma_selling_price</t>
   </si>
 </sst>
 </file>
@@ -393,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -404,18 +401,17 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="3.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1"/>
+    <col min="7" max="7" width="26.625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -426,31 +422,28 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -461,31 +454,28 @@
         <v>200</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="1">
         <v>0.99</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="3">
         <v>60</v>
-      </c>
-      <c r="G2" s="1">
-        <v>10</v>
       </c>
       <c r="H2" s="1">
         <v>0.8</v>
       </c>
       <c r="I2" s="1">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="J2" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K2" s="1">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -496,31 +486,28 @@
         <v>220</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.99</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="3">
         <v>60</v>
-      </c>
-      <c r="G3" s="1">
-        <v>10</v>
       </c>
       <c r="H3" s="1">
         <v>0.8</v>
       </c>
       <c r="I3" s="1">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K3" s="1">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -533,123 +520,144 @@
       <c r="D4" s="3">
         <v>5.5</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.99</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="3">
         <v>60</v>
-      </c>
-      <c r="G4" s="1">
-        <v>10</v>
       </c>
       <c r="H4" s="1">
         <v>0.8</v>
       </c>
       <c r="I4" s="1">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K4" s="1">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>